<commit_message>
new make has been added
</commit_message>
<xml_diff>
--- a/data/Dataset_15Jan 2.xlsx
+++ b/data/Dataset_15Jan 2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SandhyaS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandi\OneDrive\Desktop\streamlit_price_reco\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Data_IBB_Pricing" sheetId="2" r:id="rId1"/>
@@ -3306,9 +3306,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N114" sqref="N114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>